<commit_message>
Fixed Import as well as created files till 2010
</commit_message>
<xml_diff>
--- a/YearFiles/1869.xlsx
+++ b/YearFiles/1869.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -38,22 +38,7 @@
     <t>Princeton</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Rutgers</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>11/13/1869</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
 </sst>
 </file>
@@ -402,7 +387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,61 +395,38 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
         <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E2" t="n">
         <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>